<commit_message>
July Update - add studies from 07/2025
</commit_message>
<xml_diff>
--- a/taxonomy/taxonomy_studies.xlsx
+++ b/taxonomy/taxonomy_studies.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sabrina/Nextcloud/papers/vulnerability handling AI extended /analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sabrina/Nextcloud/papers/vulnerability handling AI extended /Awesome-LLM4SVD/taxonomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6CC449-AD1D-0E43-B6CF-E53CF0169539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD381610-BAAC-9643-A4B8-B462B165EA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{0CD8BF81-F5D9-B345-B2F3-1AD266DCF6BD}"/>
   </bookViews>
   <sheets>
     <sheet name="TAXONOMY" sheetId="2" r:id="rId1"/>
+    <sheet name="EXTENDED_2025_JULY" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1102">
   <si>
     <t>Link</t>
   </si>
@@ -5400,6 +5401,181 @@
   </si>
   <si>
     <t>Custom, VulSage</t>
+  </si>
+  <si>
+    <t>icozAutomatedCodeReview2025</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2507.18476</t>
+  </si>
+  <si>
+    <t>zhangBountyBenchDollarImpact2025</t>
+  </si>
+  <si>
+    <t>liCLeVeRMultimodalContrastive</t>
+  </si>
+  <si>
+    <t>sunHgtJITJustinTimeVulnerability2025</t>
+  </si>
+  <si>
+    <t>simoniImprovingLLMReasoning2025</t>
+  </si>
+  <si>
+    <t>lekssaysLLMxCPGContextAwareVulnerability2025</t>
+  </si>
+  <si>
+    <t>liOutDistributionOut2025</t>
+  </si>
+  <si>
+    <t>liRevisitingPretrainedLanguage2025</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{icozAutomatedCodeReview2025,
+      title={{Automated Code Review Using Large Language Models with Symbolic Reasoning}}, 
+      author={Busra Icoz and Goksel Biricik},
+      year={2025},
+      eprint={2507.18476},
+      archivePrefix={arXiv}}```</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2505.15216</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{zhangBountyBenchDollarImpact2025,
+      title={{BountyBench: Dollar Impact of AI Agent Attackers and Defenders on Real-World Cybersecurity Systems}}, 
+      author={Andy K. Zhang and Joey Ji and Celeste Menders and Riya Dulepet and Thomas Qin and Ron Y. Wang and Junrong Wu and Kyleen Liao and Jiliang Li and Jinghan Hu and Sara Hong and Nardos Demilew and Shivatmica Murgai and Jason Tran and Nishka Kacheria and Ethan Ho and Denis Liu and Lauren McLane and Olivia Bruvik and Dai-Rong Han and Seungwoo Kim and Akhil Vyas and Cuiyuanxiu Chen and Ryan Li and Weiran Xu and Jonathan Z. Ye and Prerit Choudhary and Siddharth M. Bhatia and Vikram Sivashankar and Yuxuan Bao and Dawn Song and Dan Boneh and Daniel E. Ho and Percy Liang},
+      year={2025},
+      eprint={2505.15216},
+      archivePrefix={arXiv}}```</t>
+  </si>
+  <si>
+    <t>Repair, Exploit</t>
+  </si>
+  <si>
+    <t>Agentic, Cot</t>
+  </si>
+  <si>
+    <t>Multi-Class, Vulnerability-Specific</t>
+  </si>
+  <si>
+    <t>https://aclanthology.org/2025.findings-acl.414/</t>
+  </si>
+  <si>
+    <t>https://github.com/yoimiya-nlp/CLeVeR</t>
+  </si>
+  <si>
+    <t>Raw, Structure-Aware</t>
+  </si>
+  <si>
+    <t>Contrastive Learning, Pre-Training, PEFT (linear probing), Adapter-Tuning</t>
+  </si>
+  <si>
+    <t>SARD, SynData, Devign, Reveal, Custom, VCLData</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/11072308</t>
+  </si>
+  <si>
+    <t>CodeJIT</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2507.03051</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{simoniImprovingLLMReasoning2025,
+      title={{Improving LLM Reasoning for Vulnerability Detection via Group Relative Policy Optimization}}, 
+      author={Marco Simoni and Aleksandar Fontana and Giulio Rossolini and Andrea Saracino},
+      year={2025},
+      eprint={2507.03051},
+      archivePrefix={arXiv}
+}```</t>
+  </si>
+  <si>
+    <t>Big-Vul, DiverseVul, CleanVul</t>
+  </si>
+  <si>
+    <t>Zero-Shot, CoT, Full-Parameter Fine-Tuning</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2507.16585</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{lekssaysLLMxCPGContextAwareVulnerability2025,
+      title={{LLMxCPG: Context-Aware Vulnerability Detection Through Code Property Graph-Guided Large Language Models}}, 
+      author={Ahmed Lekssays and Hamza Mouhcine and Khang Tran and Ting Yu and Issa Khalil},
+      year={2025},
+      eprint={2507.16585},
+      archivePrefix={arXiv}}```</t>
+  </si>
+  <si>
+    <t>FormAI, PrimeVul, SVEN, ReposVul</t>
+  </si>
+  <si>
+    <t>https://github.com/qcri/llmxcpg; https://zenodo.org/records/15614095</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2507.21817</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{liOutDistributionOut2025,
+      title={{Out of Distribution, Out of Luck: How Well Can LLMs Trained on Vulnerability Datasets Detect Top 25 CWE Weaknesses?}}, 
+      author={Yikun Li and Ngoc Tan Bui and Ting Zhang and Martin Weyssow and Chengran Yang and Xin Zhou and Jinfeng Jiang and Junkai Chen and Huihui Huang and Huu Hung Nguyen and Chiok Yew Ho and Jie Tan and Ruiyin Li and Yide Yin and Han Wei Ang and Frank Liauw and Eng Lieh Ouh and Lwin Khin Shar and David Lo},
+      year={2025},
+      eprint={2507.21817},
+      archivePrefix={arXiv}
+```</t>
+  </si>
+  <si>
+    <t>Custom, BenchVul, TitanVul</t>
+  </si>
+  <si>
+    <t>https://github.com/yikun-li/TitanVul-BenchVul</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2507.16887</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{liRevisitingPretrainedLanguage2025,
+      title={{Revisiting Pre-trained Language Models for Vulnerability Detection}}, 
+      author={Youpeng Li and Weiliang Qi and Xuyu Wang and Fuxun Yu and Xinda Wang},
+      year={2025},
+      eprint={2507.16887},
+      archivePrefix={arXiv}
+```</t>
+  </si>
+  <si>
+    <t>Zero-Shot, Few-Shot, Full-Parameter Fine-Tuning, Low-Rank Decomposition</t>
+  </si>
+  <si>
+    <t>PrimeVul, Custom</t>
+  </si>
+  <si>
+    <t>```bibtex
+@article{sunHgtJITJustinTimeVulnerability2025,
+  author={Sun, Xiaobing and Zhou, Mingxuan and Cao, Sicong and Wu, Xiaoxue and Bo, Lili and Wu, Di and Li, Bin and Xiang, Yang},
+  journal={IEEE Transactions on Dependable and Secure Computing (TDSC)}, 
+  title={{HgtJIT: Just-in-Time Vulnerability Detection Based on Heterogeneous Graph Transformer}}, 
+  year={2025},  pages={1-17},
+  doi={10.1109/TDSC.2025.3586669}}```</t>
+  </si>
+  <si>
+    <t>```bibtex
+@inproceedings{liCLeVeRMultimodalContrastive,
+    title = {{CLeVeR: Multi-modal Contrastive Learning for Vulnerability Code Representation}},
+    author = {Li, Jiayuan  and Cui, Lei  and Zhao, Sen  and Yang, Yun  and Li, Lun  and Zhu, Hongsong},
+    booktitle = {Findings of the Association for Computational Linguistics (ACL)},
+    year = {2025},
+    address = {Vienna, Austria},
+    publisher = {ACL},
+    doi = {10.18653/v1/2025.findings-acl.414},
+    pages = {7940--7951}
+}```</t>
   </si>
 </sst>
 </file>
@@ -5490,7 +5666,61 @@
     <cellStyle name="20 % - Akzent1" xfId="1" builtinId="30"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="28">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -5563,24 +5793,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}" name="Tabelle13" displayName="Tabelle13" ref="A1:L228" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="20 % - Akzent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}" name="Tabelle13" displayName="Tabelle13" ref="A1:L228" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="20 % - Akzent1">
   <autoFilter ref="A1:L228" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L228">
     <sortCondition ref="A1:A228"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A78C51B1-18F8-4146-8B26-A6F2727A511E}" name="CitationKey" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{40117DA0-BA29-6144-A98C-FFCF99C5B76B}" name="BibTeX" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{32B6540B-6321-ED46-8A5E-58EF4629F7FD}" name="Link" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{56F128CB-ACDC-E140-ADC0-591269C4979B}" name="Repo Link" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{9147C288-87B7-9947-B7BB-36B8B5E3F4FA}" name="First_Published" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{160F39B6-C7C4-A247-BF62-2755CF04A4FE}" name="Current_Version" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{9F795949-F876-6342-A0CF-90F83E0D3786}" name="Task" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{1DAEB1B2-4FC4-AF43-A46C-F1B8F40BD013}" name="Extended" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{DB4F482C-4D92-064D-9B44-1AB02DADB312}" name="Architecture" dataDxfId="3" dataCellStyle="Standard"/>
-    <tableColumn id="6" xr3:uid="{B6B3F66A-0F48-E440-8D86-2FDA6F09954C}" name="Technique" dataDxfId="2" dataCellStyle="Standard"/>
-    <tableColumn id="7" xr3:uid="{0BC3BC75-E966-A14E-B932-8535D42F32EC}" name="Input" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{FAA2202E-70BF-0C4A-9142-305BE16141E1}" name="Dataset" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A78C51B1-18F8-4146-8B26-A6F2727A511E}" name="CitationKey" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{40117DA0-BA29-6144-A98C-FFCF99C5B76B}" name="BibTeX" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{32B6540B-6321-ED46-8A5E-58EF4629F7FD}" name="Link" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{56F128CB-ACDC-E140-ADC0-591269C4979B}" name="Repo Link" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{9147C288-87B7-9947-B7BB-36B8B5E3F4FA}" name="First_Published" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{160F39B6-C7C4-A247-BF62-2755CF04A4FE}" name="Current_Version" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{9F795949-F876-6342-A0CF-90F83E0D3786}" name="Task" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{1DAEB1B2-4FC4-AF43-A46C-F1B8F40BD013}" name="Extended" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{DB4F482C-4D92-064D-9B44-1AB02DADB312}" name="Architecture" dataDxfId="17" dataCellStyle="Standard"/>
+    <tableColumn id="6" xr3:uid="{B6B3F66A-0F48-E440-8D86-2FDA6F09954C}" name="Technique" dataDxfId="16" dataCellStyle="Standard"/>
+    <tableColumn id="7" xr3:uid="{0BC3BC75-E966-A14E-B932-8535D42F32EC}" name="Input" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{FAA2202E-70BF-0C4A-9142-305BE16141E1}" name="Dataset" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ED15970-26D6-7B46-A91C-7190902B89F5}" name="Tabelle132" displayName="Tabelle132" ref="A1:L9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="20 % - Akzent1">
+  <autoFilter ref="A1:L9" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L2">
+    <sortCondition ref="A1:A2"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{256A5F0E-D4E0-6846-A3F4-2B63586D0525}" name="CitationKey" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{7026869E-E8BF-3C43-A672-81C3842B8EAA}" name="BibTeX" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{D803DA86-E9E1-FD41-912C-AC171207CF57}" name="Link" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{248692EB-E170-6548-94C9-433C79023659}" name="Repo Link" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{01AF8DCD-A5D5-B94C-91E7-BEC676FAAC6F}" name="First_Published" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{B159F186-D47D-A04C-A5F9-738EAAD562E0}" name="Current_Version" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C87916AD-A12D-A142-A331-1E65181D43E5}" name="Task" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{FDCB014B-B0AF-E240-8355-097EEFBD572F}" name="Extended" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{4B158E02-E1F1-8A4F-90FC-87CC2B87DC66}" name="Architecture" dataDxfId="3" dataCellStyle="Standard"/>
+    <tableColumn id="6" xr3:uid="{DE920C72-4815-B944-BD49-D1274EA053DB}" name="Technique" dataDxfId="2" dataCellStyle="Standard"/>
+    <tableColumn id="7" xr3:uid="{8F096544-1567-4F4F-926D-F5D56F51DA7F}" name="Input" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{C1FBC2F6-7D23-8949-8D2C-0F7A8CEC218A}" name="Dataset" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5885,8 +6139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E2F0CF-856A-D744-AC6E-C6871A5E14AF}">
   <dimension ref="A1:L228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F202" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L227" sqref="L227"/>
+    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14029,4 +14283,350 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833C8C6E-CB4E-2E48-9613-B0BA77FFC1FE}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="39.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="42.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="119.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E2" s="4">
+        <v>45862</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45862</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>331</v>
+      </c>
+      <c r="I2" t="s">
+        <v>315</v>
+      </c>
+      <c r="J2" t="s">
+        <v>440</v>
+      </c>
+      <c r="K2" t="s">
+        <v>314</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E3" s="4">
+        <v>45798</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45848</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I3" t="s">
+        <v>323</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1075</v>
+      </c>
+      <c r="K3" t="s">
+        <v>322</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E4" s="4">
+        <v>45839</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45840</v>
+      </c>
+      <c r="G4" t="s">
+        <v>313</v>
+      </c>
+      <c r="I4" t="s">
+        <v>323</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1080</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E5" s="4">
+        <v>45845</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45846</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>427</v>
+      </c>
+      <c r="J5" t="s">
+        <v>404</v>
+      </c>
+      <c r="K5" t="s">
+        <v>393</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E6" s="4">
+        <v>45841</v>
+      </c>
+      <c r="F6" s="4">
+        <v>45842</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>331</v>
+      </c>
+      <c r="I6" t="s">
+        <v>320</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1087</v>
+      </c>
+      <c r="K6" t="s">
+        <v>364</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E7" s="4">
+        <v>45860</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45860</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>320</v>
+      </c>
+      <c r="J7" t="s">
+        <v>537</v>
+      </c>
+      <c r="K7" t="s">
+        <v>395</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E8" s="4">
+        <v>45867</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45883</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
+        <v>323</v>
+      </c>
+      <c r="J8" t="s">
+        <v>436</v>
+      </c>
+      <c r="K8" t="s">
+        <v>314</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E9" s="4">
+        <v>45860</v>
+      </c>
+      <c r="F9" s="4">
+        <v>45860</v>
+      </c>
+      <c r="G9" t="s">
+        <v>313</v>
+      </c>
+      <c r="I9" t="s">
+        <v>323</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1098</v>
+      </c>
+      <c r="K9" t="s">
+        <v>395</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
August Update - add studies from 08/2025
</commit_message>
<xml_diff>
--- a/taxonomy/taxonomy_studies.xlsx
+++ b/taxonomy/taxonomy_studies.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sabrina/Nextcloud/papers/vulnerability handling AI extended /Awesome-LLM4SVD/taxonomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD381610-BAAC-9643-A4B8-B462B165EA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0D35C8-2043-C74F-A450-C6FE62DF634C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{0CD8BF81-F5D9-B345-B2F3-1AD266DCF6BD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" activeTab="2" xr2:uid="{0CD8BF81-F5D9-B345-B2F3-1AD266DCF6BD}"/>
   </bookViews>
   <sheets>
     <sheet name="TAXONOMY" sheetId="2" r:id="rId1"/>
     <sheet name="EXTENDED_2025_JULY" sheetId="4" r:id="rId2"/>
+    <sheet name="EXTENDED_2025_AUGUST" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="1127">
   <si>
     <t>Link</t>
   </si>
@@ -5577,6 +5578,125 @@
     pages = {7940--7951}
 }```</t>
   </si>
+  <si>
+    <t>gnieciakLargeLanguageModels2025</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{gnieciakLargeLanguageModels2025,
+      title={{Large Language Models Versus Static Code Analysis Tools: A Systematic Benchmark for Vulnerability Detection}}, 
+      author={Damian Gnieciak and Tomasz Szandala},
+      year={2025},
+      eprint={2508.04448},
+      archivePrefix={arXiv}}```</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/2508.04448</t>
+  </si>
+  <si>
+    <t>https://github.com/Damian0401/ProjectAnalyzer</t>
+  </si>
+  <si>
+    <t>liCryptoScopeUtilizingLarge2025</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{liCryptoScopeUtilizingLarge2025,
+      title={{CryptoScope: Utilizing Large Language Models for Automated Cryptographic Logic Vulnerability Detection}}, 
+      author={Zhihao Li and Zimo Ji and Tao Zheng and Hao Ren and Xiao Lan},
+      year={2025},
+      eprint={2508.11599},
+      archivePrefix={arXiv}
+}```</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2508.11599</t>
+  </si>
+  <si>
+    <t>LLM-CLVA</t>
+  </si>
+  <si>
+    <t>linWAADWebVulnerability2025</t>
+  </si>
+  <si>
+    <t>```bibtex
+@inproceedings{linWAADWebVulnerability2025,
+author={Lin, Xiangnan and Lu, Bin and Liu, Long and Guo, Zhongyu and Sun, Rongbo and Wang, Jiancheng},
+  booktitle={International Conference on Computer Engineering and Application (ICCEA)}, 
+  title={{WAAD: A Web Vulnerability Attack Behavior Identification Method Based on Large Language Model}}, 
+  year={2025},
+  volume={},
+  number={},
+  pages={1091-1101},
+  doi={10.1109/ICCEA65460.2025.11103444}
+}```</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/11103444</t>
+  </si>
+  <si>
+    <t>Multi-Task Learning, LoRA Derivatives, CoT, Agentic</t>
+  </si>
+  <si>
+    <t>sayaghThinkBroadAct2025</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{sayaghThinkBroadAct2025,
+      title={{Think Broad, Act Narrow: CWE Identification with Multi-Agent Large Language Models}}, 
+      author={Mohammed Sayagh and Mohammad Ghafari},
+      year={2025},
+      eprint={2508.01451},
+      archivePrefix={arXiv}
+}```</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2508.01451</t>
+  </si>
+  <si>
+    <t>https://zenodo.org/records/15871507</t>
+  </si>
+  <si>
+    <t>mhatreLLMGUARDLargeLanguage2025</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{mhatreLLMGUARDLargeLanguage2025,
+      title={{LLM-GUARD: Large Language Model-Based Detection and Repair of Bugs and Security Vulnerabilities in C++ and Python}}, 
+      author={Akshay Mhatre and Noujoud Nader and Patrick Diehl and Deepti Gupta},
+      year={2025},
+      eprint={2508.16419},
+      archivePrefix={arXiv}
+}```</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2508.16419</t>
+  </si>
+  <si>
+    <t>https://github.com/NoujoudNader/LLM-Bugs-Detection</t>
+  </si>
+  <si>
+    <t>Custom, SEED Labs, OpenSSL, PyBugHive</t>
+  </si>
+  <si>
+    <t>safdarDataContextMatter2025</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{safdarDataContextMatter2025,
+      title={{Data and Context Matter: Towards Generalizing AI-based Software Vulnerability Detection}}, 
+      author={Rijha Safdar and Danyail Mateen and Syed Taha Ali and M. Umer Ashfaq and Wajahat Hussain},
+      year={2025},
+      eprint={2508.16625},
+      archivePrefix={arXiv}
+}```</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2508.16625</t>
+  </si>
+  <si>
+    <t>Custom, Big-Vul, Linux Dataset, PrimeVul, Claude-generated</t>
+  </si>
 </sst>
 </file>
 
@@ -5585,7 +5705,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5617,8 +5737,15 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5631,6 +5758,11 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5641,11 +5773,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5661,12 +5794,70 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="20 % - Akzent1" xfId="1" builtinId="30"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="42">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -5793,48 +5984,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}" name="Tabelle13" displayName="Tabelle13" ref="A1:L228" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="20 % - Akzent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}" name="Tabelle13" displayName="Tabelle13" ref="A1:L228" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowCellStyle="20 % - Akzent1">
   <autoFilter ref="A1:L228" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L228">
     <sortCondition ref="A1:A228"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A78C51B1-18F8-4146-8B26-A6F2727A511E}" name="CitationKey" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{40117DA0-BA29-6144-A98C-FFCF99C5B76B}" name="BibTeX" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{32B6540B-6321-ED46-8A5E-58EF4629F7FD}" name="Link" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{56F128CB-ACDC-E140-ADC0-591269C4979B}" name="Repo Link" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{9147C288-87B7-9947-B7BB-36B8B5E3F4FA}" name="First_Published" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{160F39B6-C7C4-A247-BF62-2755CF04A4FE}" name="Current_Version" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{9F795949-F876-6342-A0CF-90F83E0D3786}" name="Task" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{1DAEB1B2-4FC4-AF43-A46C-F1B8F40BD013}" name="Extended" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{DB4F482C-4D92-064D-9B44-1AB02DADB312}" name="Architecture" dataDxfId="17" dataCellStyle="Standard"/>
-    <tableColumn id="6" xr3:uid="{B6B3F66A-0F48-E440-8D86-2FDA6F09954C}" name="Technique" dataDxfId="16" dataCellStyle="Standard"/>
-    <tableColumn id="7" xr3:uid="{0BC3BC75-E966-A14E-B932-8535D42F32EC}" name="Input" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{FAA2202E-70BF-0C4A-9142-305BE16141E1}" name="Dataset" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{A78C51B1-18F8-4146-8B26-A6F2727A511E}" name="CitationKey" dataDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{40117DA0-BA29-6144-A98C-FFCF99C5B76B}" name="BibTeX" dataDxfId="38"/>
+    <tableColumn id="10" xr3:uid="{32B6540B-6321-ED46-8A5E-58EF4629F7FD}" name="Link" dataDxfId="37"/>
+    <tableColumn id="12" xr3:uid="{56F128CB-ACDC-E140-ADC0-591269C4979B}" name="Repo Link" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{9147C288-87B7-9947-B7BB-36B8B5E3F4FA}" name="First_Published" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{160F39B6-C7C4-A247-BF62-2755CF04A4FE}" name="Current_Version" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{9F795949-F876-6342-A0CF-90F83E0D3786}" name="Task" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{1DAEB1B2-4FC4-AF43-A46C-F1B8F40BD013}" name="Extended" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{DB4F482C-4D92-064D-9B44-1AB02DADB312}" name="Architecture" dataDxfId="31" dataCellStyle="Standard"/>
+    <tableColumn id="6" xr3:uid="{B6B3F66A-0F48-E440-8D86-2FDA6F09954C}" name="Technique" dataDxfId="30" dataCellStyle="Standard"/>
+    <tableColumn id="7" xr3:uid="{0BC3BC75-E966-A14E-B932-8535D42F32EC}" name="Input" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{FAA2202E-70BF-0C4A-9142-305BE16141E1}" name="Dataset" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ED15970-26D6-7B46-A91C-7190902B89F5}" name="Tabelle132" displayName="Tabelle132" ref="A1:L9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="20 % - Akzent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ED15970-26D6-7B46-A91C-7190902B89F5}" name="Tabelle132" displayName="Tabelle132" ref="A1:L9" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="20 % - Akzent1">
   <autoFilter ref="A1:L9" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L2">
     <sortCondition ref="A1:A2"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{256A5F0E-D4E0-6846-A3F4-2B63586D0525}" name="CitationKey" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{7026869E-E8BF-3C43-A672-81C3842B8EAA}" name="BibTeX" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{D803DA86-E9E1-FD41-912C-AC171207CF57}" name="Link" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{248692EB-E170-6548-94C9-433C79023659}" name="Repo Link" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{01AF8DCD-A5D5-B94C-91E7-BEC676FAAC6F}" name="First_Published" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{B159F186-D47D-A04C-A5F9-738EAAD562E0}" name="Current_Version" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{C87916AD-A12D-A142-A331-1E65181D43E5}" name="Task" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{FDCB014B-B0AF-E240-8355-097EEFBD572F}" name="Extended" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{4B158E02-E1F1-8A4F-90FC-87CC2B87DC66}" name="Architecture" dataDxfId="3" dataCellStyle="Standard"/>
-    <tableColumn id="6" xr3:uid="{DE920C72-4815-B944-BD49-D1274EA053DB}" name="Technique" dataDxfId="2" dataCellStyle="Standard"/>
-    <tableColumn id="7" xr3:uid="{8F096544-1567-4F4F-926D-F5D56F51DA7F}" name="Input" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{C1FBC2F6-7D23-8949-8D2C-0F7A8CEC218A}" name="Dataset" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{256A5F0E-D4E0-6846-A3F4-2B63586D0525}" name="CitationKey" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{7026869E-E8BF-3C43-A672-81C3842B8EAA}" name="BibTeX" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{D803DA86-E9E1-FD41-912C-AC171207CF57}" name="Link" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{248692EB-E170-6548-94C9-433C79023659}" name="Repo Link" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{01AF8DCD-A5D5-B94C-91E7-BEC676FAAC6F}" name="First_Published" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{B159F186-D47D-A04C-A5F9-738EAAD562E0}" name="Current_Version" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{C87916AD-A12D-A142-A331-1E65181D43E5}" name="Task" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{FDCB014B-B0AF-E240-8355-097EEFBD572F}" name="Extended" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{4B158E02-E1F1-8A4F-90FC-87CC2B87DC66}" name="Architecture" dataDxfId="17" dataCellStyle="Standard"/>
+    <tableColumn id="6" xr3:uid="{DE920C72-4815-B944-BD49-D1274EA053DB}" name="Technique" dataDxfId="16" dataCellStyle="Standard"/>
+    <tableColumn id="7" xr3:uid="{8F096544-1567-4F4F-926D-F5D56F51DA7F}" name="Input" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{C1FBC2F6-7D23-8949-8D2C-0F7A8CEC218A}" name="Dataset" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E9B7DA3C-DCF1-A043-B2BF-96550CB5B346}" name="Tabelle1324" displayName="Tabelle1324" ref="A1:L7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="20 % - Akzent1">
+  <autoFilter ref="A1:L7" xr:uid="{E9B7DA3C-DCF1-A043-B2BF-96550CB5B346}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L5">
+    <sortCondition ref="A1:A5"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{823C6721-2163-3846-894B-67D0CB55E160}" name="CitationKey" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{59859558-F8C7-DF4E-A7E0-EE70CDC3BEC9}" name="BibTeX" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{89E1874B-C98A-964B-8B32-356C59C4D102}" name="Link" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{FF48A973-1780-AE41-AFD2-F26D2CCAC3D0}" name="Repo Link" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{5753FA1E-1855-CB49-AD57-E3734D9F8247}" name="First_Published" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{26B05692-529B-1E44-8ED2-BE1C87DFE3BA}" name="Current_Version" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{3F0DC395-4AF7-9444-9390-EDD252AEA562}" name="Task" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{BECD9A7C-03BE-CA43-BC40-BA421D8124D3}" name="Extended" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{34CF3DF5-CE25-C24A-96F4-B105F5191F17}" name="Architecture" dataDxfId="3" dataCellStyle="Standard"/>
+    <tableColumn id="6" xr3:uid="{4A27DD92-86EE-B348-A953-8D7ED77D1BE8}" name="Technique" dataDxfId="2" dataCellStyle="Standard"/>
+    <tableColumn id="7" xr3:uid="{8B05ECF3-CAB6-6644-B459-CDCF46C0F5C3}" name="Input" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{600BEC0F-4C0F-9F42-947F-06C2247F9466}" name="Dataset" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6139,7 +6354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E2F0CF-856A-D744-AC6E-C6871A5E14AF}">
   <dimension ref="A1:L228"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -14629,4 +14844,294 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12476C2-6240-214A-9F32-8A48A7261EB0}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="42.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="119.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E2" s="4">
+        <v>45875</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45875</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2" t="s">
+        <v>320</v>
+      </c>
+      <c r="J2" t="s">
+        <v>321</v>
+      </c>
+      <c r="K2" t="s">
+        <v>322</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" s="4">
+        <v>45884</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45884</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>331</v>
+      </c>
+      <c r="I3" t="s">
+        <v>320</v>
+      </c>
+      <c r="J3" t="s">
+        <v>370</v>
+      </c>
+      <c r="K3" t="s">
+        <v>322</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4" s="4">
+        <v>45772</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45882</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>331</v>
+      </c>
+      <c r="I4" t="s">
+        <v>320</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="K4" t="s">
+        <v>322</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E5" s="4">
+        <v>45871</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45871</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>337</v>
+      </c>
+      <c r="I5" t="s">
+        <v>320</v>
+      </c>
+      <c r="J5" t="s">
+        <v>386</v>
+      </c>
+      <c r="K5" t="s">
+        <v>322</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1121</v>
+      </c>
+      <c r="E6" s="4">
+        <v>45891</v>
+      </c>
+      <c r="F6" s="4">
+        <v>45891</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>331</v>
+      </c>
+      <c r="I6" t="s">
+        <v>320</v>
+      </c>
+      <c r="J6" t="s">
+        <v>321</v>
+      </c>
+      <c r="K6" t="s">
+        <v>325</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7" s="4">
+        <v>45883</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45883</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>315</v>
+      </c>
+      <c r="J7" t="s">
+        <v>436</v>
+      </c>
+      <c r="K7" t="s">
+        <v>314</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
September Update - add studies from 09/2025
</commit_message>
<xml_diff>
--- a/taxonomy/taxonomy_studies.xlsx
+++ b/taxonomy/taxonomy_studies.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sabrina/Nextcloud/papers/vulnerability handling AI extended /Awesome-LLM4SVD/taxonomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0D35C8-2043-C74F-A450-C6FE62DF634C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6049B551-7D2F-C04D-9D8A-3C588EFDBE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" activeTab="2" xr2:uid="{0CD8BF81-F5D9-B345-B2F3-1AD266DCF6BD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" activeTab="3" xr2:uid="{0CD8BF81-F5D9-B345-B2F3-1AD266DCF6BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="TAXONOMY" sheetId="2" r:id="rId1"/>
+    <sheet name="TAXONOMY_INITIAL" sheetId="2" r:id="rId1"/>
     <sheet name="EXTENDED_2025_JULY" sheetId="4" r:id="rId2"/>
     <sheet name="EXTENDED_2025_AUGUST" sheetId="5" r:id="rId3"/>
+    <sheet name="EXTENDED_2025_SEPTEMBER" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="1171">
   <si>
     <t>Link</t>
   </si>
@@ -5504,15 +5505,6 @@
     <t>https://arxiv.org/abs/2507.16585</t>
   </si>
   <si>
-    <t>```bibtex
-@preprint{lekssaysLLMxCPGContextAwareVulnerability2025,
-      title={{LLMxCPG: Context-Aware Vulnerability Detection Through Code Property Graph-Guided Large Language Models}}, 
-      author={Ahmed Lekssays and Hamza Mouhcine and Khang Tran and Ting Yu and Issa Khalil},
-      year={2025},
-      eprint={2507.16585},
-      archivePrefix={arXiv}}```</t>
-  </si>
-  <si>
     <t>FormAI, PrimeVul, SVEN, ReposVul</t>
   </si>
   <si>
@@ -5579,7 +5571,22 @@
 }```</t>
   </si>
   <si>
+    <t>sayaghThinkBroadAct2025</t>
+  </si>
+  <si>
+    <t>linWAADWebVulnerability2025</t>
+  </si>
+  <si>
+    <t>liCryptoScopeUtilizingLarge2025</t>
+  </si>
+  <si>
     <t>gnieciakLargeLanguageModels2025</t>
+  </si>
+  <si>
+    <t>https://github.com/Damian0401/ProjectAnalyzer</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/2508.04448</t>
   </si>
   <si>
     <t>```bibtex
@@ -5591,13 +5598,10 @@
       archivePrefix={arXiv}}```</t>
   </si>
   <si>
-    <t>https://arxiv.org/pdf/2508.04448</t>
-  </si>
-  <si>
-    <t>https://github.com/Damian0401/ProjectAnalyzer</t>
-  </si>
-  <si>
-    <t>liCryptoScopeUtilizingLarge2025</t>
+    <t>LLM-CLVA</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2508.11599</t>
   </si>
   <si>
     <t>```bibtex
@@ -5610,13 +5614,7 @@
 }```</t>
   </si>
   <si>
-    <t>https://arxiv.org/abs/2508.11599</t>
-  </si>
-  <si>
-    <t>LLM-CLVA</t>
-  </si>
-  <si>
-    <t>linWAADWebVulnerability2025</t>
+    <t>https://ieeexplore.ieee.org/document/11103444</t>
   </si>
   <si>
     <t>```bibtex
@@ -5632,13 +5630,10 @@
 }```</t>
   </si>
   <si>
-    <t>https://ieeexplore.ieee.org/document/11103444</t>
-  </si>
-  <si>
     <t>Multi-Task Learning, LoRA Derivatives, CoT, Agentic</t>
   </si>
   <si>
-    <t>sayaghThinkBroadAct2025</t>
+    <t>https://arxiv.org/abs/2508.01451</t>
   </si>
   <si>
     <t>```bibtex
@@ -5651,13 +5646,16 @@
 }```</t>
   </si>
   <si>
-    <t>https://arxiv.org/abs/2508.01451</t>
-  </si>
-  <si>
     <t>https://zenodo.org/records/15871507</t>
   </si>
   <si>
     <t>mhatreLLMGUARDLargeLanguage2025</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2508.16419</t>
+  </si>
+  <si>
+    <t>Custom, SEED Labs, OpenSSL, PyBugHive</t>
   </si>
   <si>
     <t>```bibtex
@@ -5670,16 +5668,16 @@
 }```</t>
   </si>
   <si>
-    <t>https://arxiv.org/abs/2508.16419</t>
-  </si>
-  <si>
     <t>https://github.com/NoujoudNader/LLM-Bugs-Detection</t>
   </si>
   <si>
-    <t>Custom, SEED Labs, OpenSSL, PyBugHive</t>
-  </si>
-  <si>
     <t>safdarDataContextMatter2025</t>
+  </si>
+  <si>
+    <t>Custom, Big-Vul, Linux Dataset, PrimeVul, Claude-generated</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2508.16625</t>
   </si>
   <si>
     <t>```bibtex
@@ -5692,10 +5690,251 @@
 }```</t>
   </si>
   <si>
-    <t>https://arxiv.org/abs/2508.16625</t>
-  </si>
-  <si>
-    <t>Custom, Big-Vul, Linux Dataset, PrimeVul, Claude-generated</t>
+    <t>alqarniAdvancedDetectionFramework2025</t>
+  </si>
+  <si>
+    <t>Low-Rank Decomposition, Multi-Task Learning</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/11153853</t>
+  </si>
+  <si>
+    <t>```bibtex
+@article{alqarniAdvancedDetectionFramework2025,
+   author={Alqarni, Mansour and Azim, Akramul},
+  journal={IEEE Access}, 
+  title={{An Advanced Detection Framework for Embedded System Vulnerabilities}}, 
+  year={2025},
+  volume={13},
+  number={},
+  pages={159207-159216},
+  doi={10.1109/ACCESS.2025.3607595}}
+}
+```</t>
+  </si>
+  <si>
+    <t>gajjarMalCodeAIAutonomousVulnerability2025a</t>
+  </si>
+  <si>
+    <t>```bibtex
+@inproceedings{gajjarMalCodeAIAutonomousVulnerability2025a,
+  author={Gajjar, Jugal and Subramaniakuppusamy, Kamalasankari and El Kachach, Noha},
+  booktitle={IEEE International Conference on Information Reuse and Integration and Data Science (IRI)}, 
+  title={{MalCodeAI: Autonomous Vulnerability Detection and Remediation via Language Agnostic Code Reasoning}}, 
+  year={2025},
+  volume={},
+  number={},
+  pages={31-36},
+  doi={10.1109/IRI66576.2025.00014}
+}
+```</t>
+  </si>
+  <si>
+    <t>Reasoning, Repair, Exploit, Severity</t>
+  </si>
+  <si>
+    <t>nganMultimodalFusionVulnerability2025</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/11133833</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/11153184</t>
+  </si>
+  <si>
+    <t>```bibtex
+@inproceedings{nganMultimodalFusionVulnerability2025,
+  author={Ngan, Nguyen Dac Thien and Khoa, Nghi Hoang and Pham, Van-Hau and Duy, Phan The},
+  booktitle={International Conference on Multimedia Analysis and Pattern Recognition (MAPR)}, 
+  title={{Multimodal Fusion for Vulnerability Detection: Integrating Sequence and Graph-Based Analysis with LLM Augmentation}}, 
+  year={2025},
+  volume={},
+  number={},
+  pages={1-6},
+  doi={10.1109/MAPR67746.2025.11133833}
+}
+```</t>
+  </si>
+  <si>
+    <t>PrimeVul, MegaVul, MegaVul+</t>
+  </si>
+  <si>
+    <t>maligazhdarovaComparativeStudyMachine2025</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/11139190</t>
+  </si>
+  <si>
+    <t>```bibtex
+@inproceedings{maligazhdarovaComparativeStudyMachine2025,
+author={Maligazhdarova, Nargiz and B. M., Avinash and Mukasheva, Assel and Yedilkhan, Didar and Askhatuly, Aidos and Berdyshev, A.},
+  booktitle={IEEE International Conference on Smart Information Systems and Technologies (SIST)}, 
+  title={{A Comparative Study of Machine Learning and Large Language Models for SQL and NoSQL Injection Vulnerability Detection}}, 
+  year={2025},
+  volume={},
+  number={},
+  pages={1-7},
+  doi={10.1109/SIST61657.2025.11139190}
+}
+```</t>
+  </si>
+  <si>
+    <t>jararwehLLaVulMultimodalLLM2025</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/11140501</t>
+  </si>
+  <si>
+    <t>DiverseVul, Custom</t>
+  </si>
+  <si>
+    <t>liMAVULMultiAgentVulnerability2025</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2510.00317</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{liMAVULMultiAgentVulnerability2025,
+      title={{MAVUL: Multi-Agent Vulnerability Detection via Contextual Reasoning and Interactive Refinement}}, 
+      author={Youpeng Li and Kartik Joshi and Xinda Wang and Eric Wong},
+      year={2025},
+      eprint={2510.00317},
+      archivePrefix={arXiv}
+}```</t>
+  </si>
+  <si>
+    <t>https://github.com/youpengl/MAVUL</t>
+  </si>
+  <si>
+    <t>JitVul (PrimeVul)</t>
+  </si>
+  <si>
+    <t>mockCrossDomainEvaluationTransformerBased2025</t>
+  </si>
+  <si>
+    <t>https://github.com/CybersecurityLab-unibz/cross_domain_evaluation</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2509.09313</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{mockCrossDomainEvaluationTransformerBased2025,
+      title={{Cross-Domain Evaluation of Transformer-Based Vulnerability Detection on Open \&amp; Industry Data}}, 
+      author={Moritz Mock and Thomas Forrer and Barbara Russo},
+      year={2025},
+      eprint={2509.09313},
+      archivePrefix={arXiv}
+}```</t>
+  </si>
+  <si>
+    <t>Devign, Reveal, Big-Vul</t>
+  </si>
+  <si>
+    <t>https://github.com/sssszh/ELVul4LLM</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2509.12629</t>
+  </si>
+  <si>
+    <t>sunEnsemblingLargeLanguage2025</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{sunEnsemblingLargeLanguage2025,
+      title={{Ensembling Large Language Models for Code Vulnerability Detection: An Empirical Evaluation}}, 
+      author={Zhihong Sun and Jia Li and Yao Wan and Chuanyi Li and Hongyu Zhang and Zhi jin and Ge Li and Hong Liu and Chen Lyu and Songlin Hu},
+      year={2025},
+      eprint={2509.12629},
+      archivePrefix={arXiv}
+}```</t>
+  </si>
+  <si>
+    <t>wangVulAgentHypothesisValidationBased2025</t>
+  </si>
+  <si>
+    <t>jiangEnhancingFineGrainedVulnerability2025</t>
+  </si>
+  <si>
+    <t>guWeaklySupervisedVulnerability2025</t>
+  </si>
+  <si>
+    <t>```bibtex
+@inproceedings{lekssaysLLMxCPGContextAwareVulnerability2025,
+      title={{LLMxCPG: Context-Aware Vulnerability Detection Through Code Property Graph-Guided Large Language Models}}, 
+      author={Ahmed Lekssays and Hamza Mouhcine and Khang Tran and Ting Yu and Issa Khalil},
+      booktitle={34th USENIX Security Symposium (USENIX Security 25)},
+  pages={489--507},
+  year={2025},
+      }```</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2509.11523</t>
+  </si>
+  <si>
+    <t>```bibtex
+@preprint{wangVulAgentHypothesisValidationBased2025,
+       title={{VulAgent: Hypothesis-Validation based Multi-Agent Vulnerability Detection}}, 
+      author={Ziliang Wang and Ge Li and Jia Li and Hao Zhu and Zhi Jin},
+      year={2025},
+      eprint={2509.11523},
+      archivePrefix={arXiv}
+}```</t>
+  </si>
+  <si>
+    <t>https://github.com/YuanJiangGit/RLFD</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/11145224</t>
+  </si>
+  <si>
+    <t>```bibtex
+@article{jiangEnhancingFineGrainedVulnerability2025,
+   author={Jiang, Yuan and Qu, Zhichen and Treude, Christoph and Su, Xiaohong and Wang, Tiantian},
+  journal={IEEE Transactions on Software Engineering (TSE)}, 
+  title={{Enhancing Fine-Grained Vulnerability Detection With Reinforcement Learning}}, 
+  year={2025},
+  volume={51},
+  number={10},
+  pages={2900-2920},
+  doi={10.1109/TSE.2025.3603400}
+}
+```</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/abs/10.1145/3768572</t>
+  </si>
+  <si>
+    <t>```bibtex
+@article{jiangEnhancingFineGrainedVulnerability2025,
+   author={Gu, Wenchao and Chen, Yupan and Wang, Yanlin and Zhang, Hongyu and Gao, Cuiyun and Lyu, Michael R.},
+  journal={ACM Transactions on Software Engineering and Methodology (TOSEM)}, 
+  title={{Weakly Supervised Vulnerability Localization via Multiple Instance Learning}}, 
+  year={2025},
+  volume={},
+  number={},
+  pages={},
+  doi={10.1145/3768572}
+}
+```</t>
+  </si>
+  <si>
+    <t>Big-Vul, ReVeal, CVEfixes, Devign</t>
+  </si>
+  <si>
+    <t>```bibtex
+@inproceedings{jararwehLLaVulMultimodalLLM2025,
+ author={Jararweh, Ala and Adams, Michael and Sahu, Avinash and Mueen, Abdullah and Anwar, Afsah},
+  booktitle={Intelligent Cybersecurity Conference (ICSC)}, 
+  title={{LLaVul: A Multimodal LLM for Interpretable Vulnerability Reasoning about Source Code}}, 
+  year={2025},
+  volume={},
+  number={},
+  pages={232-241},
+  doi={10.1109/ICSC65596.2025.11140501}
+}
+```</t>
   </si>
 </sst>
 </file>
@@ -5705,7 +5944,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5744,6 +5983,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -5773,12 +6020,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5797,13 +6045,69 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20 % - Akzent1" xfId="1" builtinId="30"/>
+    <cellStyle name="Link" xfId="3" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="56">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -5984,72 +6288,96 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}" name="Tabelle13" displayName="Tabelle13" ref="A1:L228" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowCellStyle="20 % - Akzent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}" name="Tabelle13" displayName="Tabelle13" ref="A1:L228" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" headerRowCellStyle="20 % - Akzent1">
   <autoFilter ref="A1:L228" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L228">
-    <sortCondition ref="A1:A228"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:L223">
+    <sortCondition ref="E1:E228"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A78C51B1-18F8-4146-8B26-A6F2727A511E}" name="CitationKey" dataDxfId="39"/>
-    <tableColumn id="11" xr3:uid="{40117DA0-BA29-6144-A98C-FFCF99C5B76B}" name="BibTeX" dataDxfId="38"/>
-    <tableColumn id="10" xr3:uid="{32B6540B-6321-ED46-8A5E-58EF4629F7FD}" name="Link" dataDxfId="37"/>
-    <tableColumn id="12" xr3:uid="{56F128CB-ACDC-E140-ADC0-591269C4979B}" name="Repo Link" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{9147C288-87B7-9947-B7BB-36B8B5E3F4FA}" name="First_Published" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{160F39B6-C7C4-A247-BF62-2755CF04A4FE}" name="Current_Version" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{9F795949-F876-6342-A0CF-90F83E0D3786}" name="Task" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{1DAEB1B2-4FC4-AF43-A46C-F1B8F40BD013}" name="Extended" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{DB4F482C-4D92-064D-9B44-1AB02DADB312}" name="Architecture" dataDxfId="31" dataCellStyle="Standard"/>
-    <tableColumn id="6" xr3:uid="{B6B3F66A-0F48-E440-8D86-2FDA6F09954C}" name="Technique" dataDxfId="30" dataCellStyle="Standard"/>
-    <tableColumn id="7" xr3:uid="{0BC3BC75-E966-A14E-B932-8535D42F32EC}" name="Input" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{FAA2202E-70BF-0C4A-9142-305BE16141E1}" name="Dataset" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{A78C51B1-18F8-4146-8B26-A6F2727A511E}" name="CitationKey" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{40117DA0-BA29-6144-A98C-FFCF99C5B76B}" name="BibTeX" dataDxfId="52"/>
+    <tableColumn id="10" xr3:uid="{32B6540B-6321-ED46-8A5E-58EF4629F7FD}" name="Link" dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{56F128CB-ACDC-E140-ADC0-591269C4979B}" name="Repo Link" dataDxfId="50"/>
+    <tableColumn id="9" xr3:uid="{9147C288-87B7-9947-B7BB-36B8B5E3F4FA}" name="First_Published" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{160F39B6-C7C4-A247-BF62-2755CF04A4FE}" name="Current_Version" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{9F795949-F876-6342-A0CF-90F83E0D3786}" name="Task" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{1DAEB1B2-4FC4-AF43-A46C-F1B8F40BD013}" name="Extended" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{DB4F482C-4D92-064D-9B44-1AB02DADB312}" name="Architecture" dataDxfId="45" dataCellStyle="Standard"/>
+    <tableColumn id="6" xr3:uid="{B6B3F66A-0F48-E440-8D86-2FDA6F09954C}" name="Technique" dataDxfId="44" dataCellStyle="Standard"/>
+    <tableColumn id="7" xr3:uid="{0BC3BC75-E966-A14E-B932-8535D42F32EC}" name="Input" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{FAA2202E-70BF-0C4A-9142-305BE16141E1}" name="Dataset" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ED15970-26D6-7B46-A91C-7190902B89F5}" name="Tabelle132" displayName="Tabelle132" ref="A1:L9" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="20 % - Akzent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3ED15970-26D6-7B46-A91C-7190902B89F5}" name="Tabelle132" displayName="Tabelle132" ref="A1:L9" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowCellStyle="20 % - Akzent1">
   <autoFilter ref="A1:L9" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L2">
     <sortCondition ref="A1:A2"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{256A5F0E-D4E0-6846-A3F4-2B63586D0525}" name="CitationKey" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{7026869E-E8BF-3C43-A672-81C3842B8EAA}" name="BibTeX" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{D803DA86-E9E1-FD41-912C-AC171207CF57}" name="Link" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{248692EB-E170-6548-94C9-433C79023659}" name="Repo Link" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{01AF8DCD-A5D5-B94C-91E7-BEC676FAAC6F}" name="First_Published" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{B159F186-D47D-A04C-A5F9-738EAAD562E0}" name="Current_Version" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{C87916AD-A12D-A142-A331-1E65181D43E5}" name="Task" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{FDCB014B-B0AF-E240-8355-097EEFBD572F}" name="Extended" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{4B158E02-E1F1-8A4F-90FC-87CC2B87DC66}" name="Architecture" dataDxfId="17" dataCellStyle="Standard"/>
-    <tableColumn id="6" xr3:uid="{DE920C72-4815-B944-BD49-D1274EA053DB}" name="Technique" dataDxfId="16" dataCellStyle="Standard"/>
-    <tableColumn id="7" xr3:uid="{8F096544-1567-4F4F-926D-F5D56F51DA7F}" name="Input" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{C1FBC2F6-7D23-8949-8D2C-0F7A8CEC218A}" name="Dataset" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{256A5F0E-D4E0-6846-A3F4-2B63586D0525}" name="CitationKey" dataDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{7026869E-E8BF-3C43-A672-81C3842B8EAA}" name="BibTeX" dataDxfId="38"/>
+    <tableColumn id="10" xr3:uid="{D803DA86-E9E1-FD41-912C-AC171207CF57}" name="Link" dataDxfId="37"/>
+    <tableColumn id="12" xr3:uid="{248692EB-E170-6548-94C9-433C79023659}" name="Repo Link" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{01AF8DCD-A5D5-B94C-91E7-BEC676FAAC6F}" name="First_Published" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{B159F186-D47D-A04C-A5F9-738EAAD562E0}" name="Current_Version" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{C87916AD-A12D-A142-A331-1E65181D43E5}" name="Task" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{FDCB014B-B0AF-E240-8355-097EEFBD572F}" name="Extended" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{4B158E02-E1F1-8A4F-90FC-87CC2B87DC66}" name="Architecture" dataDxfId="31" dataCellStyle="Standard"/>
+    <tableColumn id="6" xr3:uid="{DE920C72-4815-B944-BD49-D1274EA053DB}" name="Technique" dataDxfId="30" dataCellStyle="Standard"/>
+    <tableColumn id="7" xr3:uid="{8F096544-1567-4F4F-926D-F5D56F51DA7F}" name="Input" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{C1FBC2F6-7D23-8949-8D2C-0F7A8CEC218A}" name="Dataset" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E9B7DA3C-DCF1-A043-B2BF-96550CB5B346}" name="Tabelle1324" displayName="Tabelle1324" ref="A1:L7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="20 % - Akzent1">
-  <autoFilter ref="A1:L7" xr:uid="{E9B7DA3C-DCF1-A043-B2BF-96550CB5B346}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{57922CBD-710D-2047-9CF8-5709DCD1479B}" name="Tabelle1324" displayName="Tabelle1324" ref="A1:L7" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowCellStyle="20 % - Akzent1">
+  <autoFilter ref="A1:L7" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L5">
     <sortCondition ref="A1:A5"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{823C6721-2163-3846-894B-67D0CB55E160}" name="CitationKey" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{59859558-F8C7-DF4E-A7E0-EE70CDC3BEC9}" name="BibTeX" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{89E1874B-C98A-964B-8B32-356C59C4D102}" name="Link" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{FF48A973-1780-AE41-AFD2-F26D2CCAC3D0}" name="Repo Link" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{5753FA1E-1855-CB49-AD57-E3734D9F8247}" name="First_Published" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{26B05692-529B-1E44-8ED2-BE1C87DFE3BA}" name="Current_Version" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{3F0DC395-4AF7-9444-9390-EDD252AEA562}" name="Task" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{BECD9A7C-03BE-CA43-BC40-BA421D8124D3}" name="Extended" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{34CF3DF5-CE25-C24A-96F4-B105F5191F17}" name="Architecture" dataDxfId="3" dataCellStyle="Standard"/>
-    <tableColumn id="6" xr3:uid="{4A27DD92-86EE-B348-A953-8D7ED77D1BE8}" name="Technique" dataDxfId="2" dataCellStyle="Standard"/>
-    <tableColumn id="7" xr3:uid="{8B05ECF3-CAB6-6644-B459-CDCF46C0F5C3}" name="Input" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{600BEC0F-4C0F-9F42-947F-06C2247F9466}" name="Dataset" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AABCA6CB-67FB-664C-B2E3-A95D7A3611F8}" name="CitationKey" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{4A4F47D2-86E4-B54B-B1AA-0E667C29EFF2}" name="BibTeX" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{B048EDC3-C54A-2F40-9A34-B6856B88421D}" name="Link" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{BB158AD9-6A8E-8641-A579-AB32F7E8017E}" name="Repo Link" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{15CEE507-5C41-F243-A4BD-4CB7154A4382}" name="First_Published" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{584F21C3-0AA2-3442-BA47-ADDA18C58117}" name="Current_Version" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{09CD652C-CEFE-5445-A137-AE39D88985AF}" name="Task" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{09BD2A24-4105-7047-B0C6-85502EAB1D78}" name="Extended" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{D57234C4-BD46-2E43-9C7C-BEB5370313E0}" name="Architecture" dataDxfId="17" dataCellStyle="Standard"/>
+    <tableColumn id="6" xr3:uid="{91FA0119-0F95-7C49-96D9-B3749047CD1F}" name="Technique" dataDxfId="16" dataCellStyle="Standard"/>
+    <tableColumn id="7" xr3:uid="{898B4CB9-2CFB-C44A-90ED-F65BC7BFAD8E}" name="Input" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{0BD0CAE7-5C4F-E94C-AB6C-84842B74A288}" name="Dataset" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{83FA8FFA-B77E-6448-83CF-1BAA1ED50E32}" name="Tabelle13246" displayName="Tabelle13246" ref="A1:L12" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="20 % - Akzent1">
+  <autoFilter ref="A1:L12" xr:uid="{1442EDCD-289D-E345-92D7-2EACE02AB972}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L4">
+    <sortCondition ref="A1:A4"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{AA29C645-562D-5345-959F-D559BD4A3AE9}" name="CitationKey" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{76E89C78-6CD1-CD47-A822-873618A22483}" name="BibTeX" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{692E4E75-6579-C24F-B092-D775A6AC02DD}" name="Link" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{BD55A34D-F089-3243-880A-3CBF0E67AA49}" name="Repo Link" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{96BF5171-0D80-7E40-B722-8F1C016C1D41}" name="First_Published" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{07F337D7-2E55-D542-A00E-32B772A028CE}" name="Current_Version" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{44E6C415-EA52-824D-AD81-BB67049E7FAA}" name="Task" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{61266597-E332-D34E-9B89-8D3ED0F98E07}" name="Extended" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{86A52A07-D273-EF40-98D5-F6643F1CC64C}" name="Architecture" dataDxfId="3" dataCellStyle="Standard"/>
+    <tableColumn id="6" xr3:uid="{2F0C3D62-DCF4-7847-AA8C-B38BAB9B71C6}" name="Technique" dataDxfId="2" dataCellStyle="Standard"/>
+    <tableColumn id="7" xr3:uid="{CF26C250-650E-674E-AF50-1FDF3A29D249}" name="Input" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{24C3403E-8467-B943-AFCC-65012374B954}" name="Dataset" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6355,7 +6683,7 @@
   <dimension ref="A1:L228"/>
   <sheetViews>
     <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D219" sqref="D219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6370,7 +6698,7 @@
     <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="39.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="33.6640625" style="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -6809,38 +7137,36 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>215</v>
+        <v>250</v>
       </c>
       <c r="B13" t="s">
-        <v>885</v>
+        <v>947</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" t="s">
-        <v>577</v>
-      </c>
+        <v>696</v>
+      </c>
+      <c r="D13"/>
       <c r="E13" s="4">
-        <v>45432</v>
+        <v>45156</v>
       </c>
       <c r="F13" s="4">
-        <v>45432</v>
+        <v>45156</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="s">
         <v>320</v>
       </c>
       <c r="J13" t="s">
-        <v>385</v>
+        <v>334</v>
       </c>
       <c r="K13" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="L13" t="s">
-        <v>421</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -7627,29 +7953,25 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>267</v>
+        <v>213</v>
       </c>
       <c r="B36" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>606</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D36"/>
       <c r="E36" s="4">
-        <v>45460</v>
+        <v>45293</v>
       </c>
       <c r="F36" s="4">
-        <v>45825</v>
+        <v>45335</v>
       </c>
       <c r="G36" t="s">
         <v>4</v>
       </c>
-      <c r="H36" t="s">
-        <v>343</v>
-      </c>
+      <c r="H36"/>
       <c r="I36" t="s">
         <v>320</v>
       </c>
@@ -7660,7 +7982,7 @@
         <v>322</v>
       </c>
       <c r="L36" t="s">
-        <v>1028</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -9087,36 +9409,40 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>140</v>
+        <v>216</v>
       </c>
       <c r="B77" t="s">
-        <v>664</v>
-      </c>
-      <c r="C77" t="s">
-        <v>44</v>
-      </c>
-      <c r="D77"/>
+        <v>790</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>789</v>
+      </c>
       <c r="E77" s="4">
-        <v>45559</v>
+        <v>45320</v>
       </c>
       <c r="F77" s="4">
-        <v>45618</v>
+        <v>45815</v>
       </c>
       <c r="G77" t="s">
-        <v>36</v>
-      </c>
-      <c r="H77"/>
+        <v>313</v>
+      </c>
+      <c r="H77" t="s">
+        <v>331</v>
+      </c>
       <c r="I77" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="J77" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="K77" t="s">
         <v>322</v>
       </c>
       <c r="L77" t="s">
-        <v>368</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
@@ -9299,38 +9625,38 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="B83" t="s">
-        <v>935</v>
+        <v>950</v>
       </c>
       <c r="C83" t="s">
-        <v>671</v>
-      </c>
-      <c r="D83"/>
+        <v>705</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>706</v>
+      </c>
       <c r="E83" s="4">
-        <v>45470</v>
+        <v>45377</v>
       </c>
       <c r="F83" s="4">
-        <v>45729</v>
+        <v>45377</v>
       </c>
       <c r="G83" t="s">
-        <v>4</v>
-      </c>
-      <c r="H83" t="s">
-        <v>326</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="H83"/>
       <c r="I83" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J83" t="s">
-        <v>334</v>
+        <v>448</v>
       </c>
       <c r="K83" t="s">
-        <v>322</v>
+        <v>396</v>
       </c>
       <c r="L83" t="s">
-        <v>1036</v>
+        <v>417</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
@@ -9691,38 +10017,36 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>476</v>
+        <v>274</v>
       </c>
       <c r="B94" t="s">
-        <v>686</v>
+        <v>822</v>
       </c>
       <c r="C94" t="s">
-        <v>685</v>
+        <v>90</v>
       </c>
       <c r="D94"/>
       <c r="E94" s="4">
-        <v>45829</v>
+        <v>45406</v>
       </c>
       <c r="F94" s="4">
-        <v>45829</v>
+        <v>45406</v>
       </c>
       <c r="G94" t="s">
         <v>4</v>
       </c>
-      <c r="H94" t="s">
-        <v>331</v>
-      </c>
+      <c r="H94"/>
       <c r="I94" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="J94" t="s">
-        <v>334</v>
+        <v>445</v>
       </c>
       <c r="K94" t="s">
-        <v>393</v>
+        <v>328</v>
       </c>
       <c r="L94" t="s">
-        <v>507</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
@@ -9941,36 +10265,38 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>250</v>
+        <v>166</v>
       </c>
       <c r="B101" t="s">
-        <v>947</v>
-      </c>
-      <c r="C101" t="s">
-        <v>696</v>
-      </c>
-      <c r="D101"/>
+        <v>1005</v>
+      </c>
+      <c r="C101"/>
+      <c r="D101" s="8" t="s">
+        <v>841</v>
+      </c>
       <c r="E101" s="4">
-        <v>45156</v>
+        <v>45414</v>
       </c>
       <c r="F101" s="4">
-        <v>45156</v>
+        <v>45580</v>
       </c>
       <c r="G101" t="s">
         <v>4</v>
       </c>
-      <c r="H101"/>
+      <c r="H101" t="s">
+        <v>331</v>
+      </c>
       <c r="I101" t="s">
         <v>320</v>
       </c>
       <c r="J101" t="s">
-        <v>334</v>
+        <v>543</v>
       </c>
       <c r="K101" t="s">
-        <v>325</v>
+        <v>364</v>
       </c>
       <c r="L101" t="s">
-        <v>5</v>
+        <v>416</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.2">
@@ -10159,38 +10485,38 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="B107" t="s">
-        <v>950</v>
-      </c>
-      <c r="C107" t="s">
-        <v>705</v>
+        <v>885</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="D107" t="s">
-        <v>706</v>
+        <v>577</v>
       </c>
       <c r="E107" s="4">
-        <v>45377</v>
+        <v>45432</v>
       </c>
       <c r="F107" s="4">
-        <v>45377</v>
+        <v>45432</v>
       </c>
       <c r="G107" t="s">
-        <v>313</v>
+        <v>36</v>
       </c>
       <c r="H107"/>
       <c r="I107" t="s">
         <v>320</v>
       </c>
       <c r="J107" t="s">
-        <v>448</v>
+        <v>385</v>
       </c>
       <c r="K107" t="s">
-        <v>396</v>
+        <v>322</v>
       </c>
       <c r="L107" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.2">
@@ -10441,25 +10767,29 @@
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>213</v>
+        <v>267</v>
       </c>
       <c r="B115" t="s">
-        <v>878</v>
-      </c>
-      <c r="C115" t="s">
-        <v>66</v>
-      </c>
-      <c r="D115"/>
+        <v>879</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>606</v>
+      </c>
       <c r="E115" s="4">
-        <v>45293</v>
+        <v>45460</v>
       </c>
       <c r="F115" s="4">
-        <v>45335</v>
+        <v>45825</v>
       </c>
       <c r="G115" t="s">
         <v>4</v>
       </c>
-      <c r="H115"/>
+      <c r="H115" t="s">
+        <v>343</v>
+      </c>
       <c r="I115" t="s">
         <v>320</v>
       </c>
@@ -10470,7 +10800,7 @@
         <v>322</v>
       </c>
       <c r="L115" t="s">
-        <v>335</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
@@ -11115,38 +11445,38 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B134" t="s">
-        <v>741</v>
+        <v>935</v>
       </c>
       <c r="C134" t="s">
-        <v>54</v>
+        <v>671</v>
       </c>
       <c r="D134"/>
       <c r="E134" s="4">
-        <v>45504</v>
+        <v>45470</v>
       </c>
       <c r="F134" s="4">
-        <v>45504</v>
+        <v>45729</v>
       </c>
       <c r="G134" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="H134" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="I134" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="J134" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="K134" t="s">
         <v>322</v>
       </c>
       <c r="L134" t="s">
-        <v>32</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.2">
@@ -11641,40 +11971,38 @@
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>484</v>
+        <v>133</v>
       </c>
       <c r="B149" t="s">
-        <v>761</v>
+        <v>741</v>
       </c>
       <c r="C149" t="s">
-        <v>759</v>
-      </c>
-      <c r="D149" t="s">
-        <v>760</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D149"/>
       <c r="E149" s="4">
-        <v>45784</v>
+        <v>45504</v>
       </c>
       <c r="F149" s="4">
-        <v>45784</v>
+        <v>45504</v>
       </c>
       <c r="G149" t="s">
-        <v>327</v>
+        <v>36</v>
       </c>
       <c r="H149" t="s">
-        <v>343</v>
+        <v>318</v>
       </c>
       <c r="I149" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J149" t="s">
-        <v>515</v>
+        <v>347</v>
       </c>
       <c r="K149" t="s">
         <v>322</v>
       </c>
       <c r="L149" t="s">
-        <v>1025</v>
+        <v>32</v>
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.2">
@@ -11715,36 +12043,38 @@
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>218</v>
+        <v>140</v>
       </c>
       <c r="B151" t="s">
-        <v>977</v>
+        <v>664</v>
       </c>
       <c r="C151" t="s">
-        <v>764</v>
+        <v>44</v>
       </c>
       <c r="D151"/>
       <c r="E151" s="4">
-        <v>45606</v>
+        <v>45559</v>
       </c>
       <c r="F151" s="4">
         <v>45618</v>
       </c>
       <c r="G151" t="s">
-        <v>4</v>
-      </c>
-      <c r="H151"/>
+        <v>36</v>
+      </c>
+      <c r="H151" t="s">
+        <v>337</v>
+      </c>
       <c r="I151" t="s">
         <v>320</v>
       </c>
       <c r="J151" t="s">
-        <v>370</v>
+        <v>334</v>
       </c>
       <c r="K151" t="s">
         <v>322</v>
       </c>
       <c r="L151" t="s">
-        <v>97</v>
+        <v>368</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.2">
@@ -11821,38 +12151,36 @@
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>381</v>
+        <v>218</v>
       </c>
       <c r="B154" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="C154" t="s">
-        <v>769</v>
-      </c>
-      <c r="D154" t="s">
-        <v>770</v>
-      </c>
+        <v>764</v>
+      </c>
+      <c r="D154"/>
       <c r="E154" s="4">
-        <v>45635</v>
+        <v>45606</v>
       </c>
       <c r="F154" s="4">
-        <v>45635</v>
+        <v>45618</v>
       </c>
       <c r="G154" t="s">
         <v>4</v>
       </c>
       <c r="H154"/>
       <c r="I154" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J154" t="s">
-        <v>453</v>
+        <v>370</v>
       </c>
       <c r="K154" t="s">
         <v>322</v>
       </c>
       <c r="L154" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.2">
@@ -12283,40 +12611,38 @@
     </row>
     <row r="167" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>216</v>
+        <v>381</v>
       </c>
       <c r="B167" t="s">
-        <v>790</v>
+        <v>980</v>
       </c>
       <c r="C167" t="s">
-        <v>69</v>
+        <v>769</v>
       </c>
       <c r="D167" t="s">
-        <v>789</v>
+        <v>770</v>
       </c>
       <c r="E167" s="4">
-        <v>45320</v>
+        <v>45635</v>
       </c>
       <c r="F167" s="4">
-        <v>45815</v>
+        <v>45635</v>
       </c>
       <c r="G167" t="s">
-        <v>313</v>
-      </c>
-      <c r="H167" t="s">
-        <v>331</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="H167"/>
       <c r="I167" t="s">
         <v>323</v>
       </c>
       <c r="J167" t="s">
-        <v>354</v>
+        <v>453</v>
       </c>
       <c r="K167" t="s">
         <v>322</v>
       </c>
       <c r="L167" t="s">
-        <v>1025</v>
+        <v>104</v>
       </c>
     </row>
     <row r="168" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -13107,36 +13433,38 @@
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="B190" t="s">
-        <v>822</v>
-      </c>
-      <c r="C190" t="s">
-        <v>90</v>
-      </c>
-      <c r="D190"/>
+        <v>857</v>
+      </c>
+      <c r="C190" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D190" t="s">
+        <v>858</v>
+      </c>
       <c r="E190" s="4">
-        <v>45406</v>
+        <v>45719</v>
       </c>
       <c r="F190" s="4">
-        <v>45406</v>
+        <v>45719</v>
       </c>
       <c r="G190" t="s">
         <v>4</v>
       </c>
       <c r="H190"/>
       <c r="I190" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="J190" t="s">
-        <v>445</v>
+        <v>556</v>
       </c>
       <c r="K190" t="s">
         <v>328</v>
       </c>
       <c r="L190" t="s">
-        <v>1055</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.2">
@@ -13499,23 +13827,23 @@
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>166</v>
+        <v>498</v>
       </c>
       <c r="B201" t="s">
-        <v>1005</v>
-      </c>
-      <c r="C201"/>
-      <c r="D201" t="s">
-        <v>841</v>
-      </c>
+        <v>1018</v>
+      </c>
+      <c r="C201" t="s">
+        <v>870</v>
+      </c>
+      <c r="D201"/>
       <c r="E201" s="4">
-        <v>45414</v>
+        <v>45758</v>
       </c>
       <c r="F201" s="4">
-        <v>45580</v>
+        <v>45758</v>
       </c>
       <c r="G201" t="s">
-        <v>4</v>
+        <v>327</v>
       </c>
       <c r="H201" t="s">
         <v>331</v>
@@ -13524,13 +13852,13 @@
         <v>320</v>
       </c>
       <c r="J201" t="s">
-        <v>543</v>
+        <v>370</v>
       </c>
       <c r="K201" t="s">
-        <v>364</v>
+        <v>322</v>
       </c>
       <c r="L201" t="s">
-        <v>416</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.2">
@@ -13931,35 +14259,37 @@
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>288</v>
+        <v>484</v>
       </c>
       <c r="B213" t="s">
-        <v>857</v>
+        <v>761</v>
       </c>
       <c r="C213" t="s">
-        <v>289</v>
-      </c>
-      <c r="D213" t="s">
-        <v>858</v>
+        <v>759</v>
+      </c>
+      <c r="D213" s="8" t="s">
+        <v>760</v>
       </c>
       <c r="E213" s="4">
-        <v>45719</v>
+        <v>45784</v>
       </c>
       <c r="F213" s="4">
-        <v>45719</v>
+        <v>45784</v>
       </c>
       <c r="G213" t="s">
-        <v>4</v>
-      </c>
-      <c r="H213"/>
+        <v>327</v>
+      </c>
+      <c r="H213" t="s">
+        <v>343</v>
+      </c>
       <c r="I213" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="J213" t="s">
-        <v>556</v>
+        <v>515</v>
       </c>
       <c r="K213" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="L213" t="s">
         <v>1025</v>
@@ -14281,23 +14611,23 @@
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>498</v>
+        <v>476</v>
       </c>
       <c r="B223" t="s">
-        <v>1018</v>
+        <v>686</v>
       </c>
       <c r="C223" t="s">
-        <v>870</v>
+        <v>685</v>
       </c>
       <c r="D223"/>
       <c r="E223" s="4">
-        <v>45758</v>
+        <v>45829</v>
       </c>
       <c r="F223" s="4">
-        <v>45758</v>
+        <v>45829</v>
       </c>
       <c r="G223" t="s">
-        <v>327</v>
+        <v>4</v>
       </c>
       <c r="H223" t="s">
         <v>331</v>
@@ -14306,13 +14636,13 @@
         <v>320</v>
       </c>
       <c r="J223" t="s">
-        <v>370</v>
+        <v>334</v>
       </c>
       <c r="K223" t="s">
-        <v>322</v>
+        <v>393</v>
       </c>
       <c r="L223" t="s">
-        <v>1025</v>
+        <v>507</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.2">
@@ -14493,9 +14823,19 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D83" r:id="rId1" xr:uid="{C5ECA27C-1DC9-8A41-A9E1-7E0194D8A59A}"/>
+    <hyperlink ref="D213" r:id="rId2" xr:uid="{F549915A-AED1-744C-B11F-09FB6D6CA822}"/>
+    <hyperlink ref="D101" r:id="rId3" xr:uid="{8C4C9D11-822F-A64F-8E4C-2BCAB564AE88}"/>
+    <hyperlink ref="D77" r:id="rId4" xr:uid="{920A941F-8320-824D-9F25-BA8199E91F8C}"/>
+    <hyperlink ref="C77" r:id="rId5" xr:uid="{02EDB4C8-75C2-AE42-B0DA-4702903D3677}"/>
+    <hyperlink ref="C115" r:id="rId6" xr:uid="{E1D44462-CDCE-F54A-B2D5-EAD258472A3E}"/>
+    <hyperlink ref="C190" r:id="rId7" xr:uid="{770F5E06-CCEF-BF47-8D75-7C1B186A4611}"/>
+    <hyperlink ref="C107" r:id="rId8" xr:uid="{C00746B1-BA41-6542-A8C8-14DA349FCA67}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -14504,8 +14844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833C8C6E-CB4E-2E48-9613-B0BA77FFC1FE}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14639,7 +14979,7 @@
         <v>1065</v>
       </c>
       <c r="B4" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C4" t="s">
         <v>1077</v>
@@ -14674,7 +15014,7 @@
         <v>1066</v>
       </c>
       <c r="B5" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C5" t="s">
         <v>1082</v>
@@ -14741,13 +15081,13 @@
         <v>1068</v>
       </c>
       <c r="B7" t="s">
-        <v>1089</v>
+        <v>1161</v>
       </c>
       <c r="C7" t="s">
         <v>1088</v>
       </c>
       <c r="D7" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E7" s="4">
         <v>45860</v>
@@ -14768,7 +15108,7 @@
         <v>395</v>
       </c>
       <c r="L7" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="8" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
@@ -14776,13 +15116,13 @@
         <v>1069</v>
       </c>
       <c r="B8" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C8" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D8" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E8" s="4">
         <v>45867</v>
@@ -14803,7 +15143,7 @@
         <v>314</v>
       </c>
       <c r="L8" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="9" spans="1:12" customFormat="1" x14ac:dyDescent="0.2">
@@ -14811,10 +15151,10 @@
         <v>1070</v>
       </c>
       <c r="B9" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C9" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E9" s="4">
         <v>45860</v>
@@ -14829,13 +15169,13 @@
         <v>323</v>
       </c>
       <c r="J9" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="K9" t="s">
         <v>395</v>
       </c>
       <c r="L9" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
   </sheetData>
@@ -14847,11 +15187,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12476C2-6240-214A-9F32-8A48A7261EB0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94562821-7419-3149-A7C9-6097D08124C5}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14912,13 +15252,13 @@
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="B2" t="s">
-        <v>1103</v>
+        <v>1107</v>
       </c>
       <c r="C2" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="D2" t="s">
         <v>1105</v>
@@ -14948,13 +15288,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="B3" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="C3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="D3"/>
       <c r="E3" s="4">
@@ -14979,18 +15319,18 @@
         <v>322</v>
       </c>
       <c r="L3" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1110</v>
+        <v>1102</v>
       </c>
       <c r="B4" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C4" t="s">
         <v>1111</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1112</v>
       </c>
       <c r="D4"/>
       <c r="E4" s="4">
@@ -15020,16 +15360,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1114</v>
+        <v>1101</v>
       </c>
       <c r="B5" t="s">
         <v>1115</v>
       </c>
       <c r="C5" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D5" t="s">
         <v>1116</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1117</v>
       </c>
       <c r="E5" s="4">
         <v>45871</v>
@@ -15053,18 +15393,18 @@
         <v>322</v>
       </c>
       <c r="L5" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C6" t="s">
         <v>1118</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1119</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1120</v>
       </c>
       <c r="D6" t="s">
         <v>1121</v>
@@ -15091,18 +15431,18 @@
         <v>325</v>
       </c>
       <c r="L6" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B7" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C7" t="s">
         <v>1124</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1125</v>
       </c>
       <c r="D7"/>
       <c r="E7" s="4">
@@ -15125,7 +15465,473 @@
         <v>314</v>
       </c>
       <c r="L7" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE78E20B-9B3A-E34D-9DFC-82E5FB609146}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="42.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="119.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1126</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2" s="4">
+        <v>45909</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45909</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2" t="s">
+        <v>320</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="K2" t="s">
+        <v>314</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" s="4">
+        <v>45875</v>
+      </c>
+      <c r="F3" s="4">
+        <v>45875</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="I3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J3" t="s">
+        <v>537</v>
+      </c>
+      <c r="K3" t="s">
+        <v>393</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4" s="4">
+        <v>45883</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45883</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4" t="s">
+        <v>427</v>
+      </c>
+      <c r="J4" t="s">
+        <v>436</v>
+      </c>
+      <c r="K4" t="s">
+        <v>393</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5" s="4">
+        <v>45791</v>
+      </c>
+      <c r="F5" s="4">
+        <v>45791</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5" t="s">
+        <v>320</v>
+      </c>
+      <c r="J5" t="s">
+        <v>438</v>
+      </c>
+      <c r="K5" t="s">
+        <v>328</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6" s="4">
+        <v>45796</v>
+      </c>
+      <c r="F6" s="4">
+        <v>45796</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>331</v>
+      </c>
+      <c r="I6" t="s">
+        <v>323</v>
+      </c>
+      <c r="J6" t="s">
+        <v>537</v>
+      </c>
+      <c r="K6" t="s">
+        <v>314</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E7" s="4">
+        <v>45930</v>
+      </c>
+      <c r="F7" s="4">
+        <v>45901</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>331</v>
+      </c>
+      <c r="I7" t="s">
+        <v>320</v>
+      </c>
+      <c r="J7" t="s">
+        <v>386</v>
+      </c>
+      <c r="K7" t="s">
+        <v>322</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E8" s="4">
+        <v>45911</v>
+      </c>
+      <c r="F8" s="4">
+        <v>45911</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>318</v>
+      </c>
+      <c r="I8" t="s">
+        <v>315</v>
+      </c>
+      <c r="J8" t="s">
+        <v>436</v>
+      </c>
+      <c r="K8" t="s">
+        <v>314</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E9" s="4">
+        <v>45916</v>
+      </c>
+      <c r="F9" s="4">
+        <v>45918</v>
+      </c>
+      <c r="G9" t="s">
+        <v>313</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9" t="s">
+        <v>315</v>
+      </c>
+      <c r="J9" t="s">
+        <v>537</v>
+      </c>
+      <c r="K9" t="s">
+        <v>314</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10" s="4">
+        <v>45915</v>
+      </c>
+      <c r="F10" s="4">
+        <v>45915</v>
+      </c>
+      <c r="G10" t="s">
+        <v>327</v>
+      </c>
+      <c r="H10" t="s">
+        <v>331</v>
+      </c>
+      <c r="I10" t="s">
+        <v>320</v>
+      </c>
+      <c r="J10" t="s">
+        <v>386</v>
+      </c>
+      <c r="K10" t="s">
+        <v>395</v>
+      </c>
+      <c r="L10" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E11" s="4">
+        <v>45898</v>
+      </c>
+      <c r="F11" s="4">
+        <v>45898</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11" t="s">
+        <v>315</v>
+      </c>
+      <c r="J11" t="s">
+        <v>436</v>
+      </c>
+      <c r="K11" t="s">
+        <v>314</v>
+      </c>
+      <c r="L11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12" s="4">
+        <v>45914</v>
+      </c>
+      <c r="F12" s="4">
+        <v>45929</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>318</v>
+      </c>
+      <c r="I12" t="s">
+        <v>320</v>
+      </c>
+      <c r="J12" t="s">
+        <v>436</v>
+      </c>
+      <c r="K12" t="s">
+        <v>314</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>